<commit_message>
24-11-2022: Aalborg  constraints bug fix, genral bug fix, Enerplan 15.1 for Aalborg
</commit_message>
<xml_diff>
--- a/ESD_AAlborg.xlsx
+++ b/ESD_AAlborg.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>PEF_i^el</t>
   </si>
@@ -80,18 +80,39 @@
     <t>ESD</t>
   </si>
   <si>
-    <t>ESD_mod</t>
+    <t>TWh</t>
   </si>
   <si>
-    <t>TWh</t>
+    <t>is discarded from ESD because import is simply assumed NG-based condensing power. So, in the above equation import is considered twice as import and as NGS.</t>
+  </si>
+  <si>
+    <t>production (TWh)</t>
+  </si>
+  <si>
+    <t>Local PEF caculation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -119,8 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1282,10 +1307,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7131325" cy="618759"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1297,7 +1322,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6850380" y="2560320"/>
+              <a:off x="6614160" y="3040380"/>
               <a:ext cx="7131325" cy="618759"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2016,7 +2041,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="6850380" y="2560320"/>
+              <a:off x="6614160" y="3040380"/>
               <a:ext cx="7131325" cy="618759"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2100,6 +2125,233 @@
                 <a:t> )</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1500"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="679610" cy="184922"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6758940" y="2350770"/>
+              <a:ext cx="679610" cy="184922"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑒</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="FF0000"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="FF0000"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑙</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="FF0000"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑥</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t> </m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:solidFill>
+                          <a:srgbClr val="FF0000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑃𝐸</m:t>
+                    </m:r>
+                    <m:sSubSup>
+                      <m:sSubSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="FF0000"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="FF0000"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐹</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="FF0000"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖</m:t>
+                        </m:r>
+                      </m:sub>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:solidFill>
+                              <a:srgbClr val="FF0000"/>
+                            </a:solidFill>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑒𝑙</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSubSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6758940" y="2350770"/>
+              <a:ext cx="679610" cy="184922"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑒𝑙_𝑖 𝑥 𝑃𝐸𝐹_𝑖^𝑒𝑙</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -2373,23 +2625,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2397,7 +2651,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2406,7 +2660,7 @@
         <v>2.1276595744680851</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2414,7 +2668,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2422,15 +2676,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" t="s">
         <v>14</v>
       </c>
@@ -2438,7 +2698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2456,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2477,12 +2737,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
-        <f>(G8*I8+G9*I9+G10*I10)/B8</f>
+        <f>H12</f>
         <v>1.3070242656449551</v>
       </c>
       <c r="F10" t="s">
@@ -2499,7 +2759,7 @@
         <v>1.8518518518518516</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2507,15 +2767,22 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12">
         <v>0.5</v>
       </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <f>(G8*I8+G9*I9+G10*I10)/B8</f>
+        <v>1.3070242656449551</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2523,40 +2790,29 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <f>(B2*B3+B4+B5+B6)/((B8-B9)*B10+B2*B3+B4+B11+B12+(B13-(B13/B14)))</f>
-        <v>0.23874698973433423</v>
+      <c r="M14" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <f>(B4+B5+B6)/((B8-B9)*B10+B4+B11+B12+(B13-(B13/B14)))</f>
         <v>0.13611632379823704</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <f>(B4+B5+B6)/((B8-B9)*B10+B4+B11+B12+(B13-(B13/B14)))</f>
-        <v>0.13611632379823704</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
25-11-2022: Aalborg EnagyPLAN 15.1 path fixed, ESD calculation bug fixed
</commit_message>
<xml_diff>
--- a/ESD_AAlborg.xlsx
+++ b/ESD_AAlborg.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>PEF_i^el</t>
   </si>
@@ -90,6 +91,12 @@
   </si>
   <si>
     <t>Local PEF caculation</t>
+  </si>
+  <si>
+    <t>pv</t>
+  </si>
+  <si>
+    <t>Offshore</t>
   </si>
 </sst>
 </file>
@@ -1313,8 +1320,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="7131325" cy="618759"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -2033,7 +2040,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -2140,8 +2147,8 @@
       <xdr:rowOff>156210</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="679610" cy="184922"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -2177,6 +2184,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2306,7 +2314,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -2628,7 +2636,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2665,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.57999999999999996</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -2703,14 +2711,14 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <f>1.23+0.1+0.12</f>
-        <v>1.4500000000000002</v>
+        <f>SUM(G8:G12)</f>
+        <v>1.52</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
       <c r="G8">
-        <v>1.23</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2721,13 +2729,13 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.16</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="G9">
-        <v>0.12</v>
+        <v>0.3</v>
       </c>
       <c r="H9">
         <v>0.25</v>
@@ -2742,8 +2750,8 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <f>H12</f>
-        <v>1.3070242656449551</v>
+        <f>H15</f>
+        <v>1.6481481481481479</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -2764,7 +2772,16 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>1.3</v>
+        <v>1.52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11">
+        <v>0.53</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -2774,12 +2791,14 @@
       <c r="B12">
         <v>0.5</v>
       </c>
-      <c r="G12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <f>(G8*I8+G9*I9+G10*I10)/B8</f>
-        <v>1.3070242656449551</v>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>0.02</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2787,7 +2806,7 @@
         <v>8</v>
       </c>
       <c r="B13">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -2801,13 +2820,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <f>(G8*I8+G9*I9+G10*I10+G11*I11+G12*I12)/B8</f>
+        <v>1.6481481481481479</v>
+      </c>
+    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <f>(B4+B5+B6)/((B8-B9)*B10+B4+B11+B12+(B13-(B13/B14)))</f>
-        <v>0.13611632379823704</v>
+        <v>0.10634847080630214</v>
       </c>
     </row>
   </sheetData>
@@ -2815,4 +2843,197 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <f>1/0.47</f>
+        <v>2.1276595744680851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>0.67</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1.07</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>0.04</v>
+      </c>
+      <c r="H9">
+        <v>0.25</v>
+      </c>
+      <c r="I9">
+        <f>1/H9</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <f>H12</f>
+        <v>1.2533150434385001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>0.54</v>
+      </c>
+      <c r="I10">
+        <f>1/H10</f>
+        <v>1.8518518518518516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <f>(G8*I8+G9*I9+G10*I10)/B8</f>
+        <v>1.2533150434385001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f>(B4+B5+B6)/((B8-B9)*B10+B4+B11+B12+(B13-(B13/B14)))</f>
+        <v>2.4611610333050114E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <f xml:space="preserve"> G8*1 + G9 * (1/0.25) + G10 * (1/0.54)</f>
+        <v>1.0151851851851852</v>
+      </c>
+      <c r="H20">
+        <f>1/0.25</f>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>